<commit_message>
update bug fixed report finance
</commit_message>
<xml_diff>
--- a/uploads/finance/Template_report.xlsx
+++ b/uploads/finance/Template_report.xlsx
@@ -12,10 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="03 Sept 18" sheetId="2" r:id="rId1"/>
+    <sheet name="Rekap" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'03 Sept 18'!$A$5:$J$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Rekap!$A$5:$J$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -180,33 +180,33 @@
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -492,21 +492,21 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="9"/>
-    <col min="2" max="2" width="33.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="9" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="33.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="4" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -525,58 +525,58 @@
       </c>
     </row>
     <row r="4" spans="1:10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:10" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:10" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="6" t="s">
+    <row r="6" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="5"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D9" s="11"/>
+      <c r="D9" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>